<commit_message>
added strong/weak foot and updated to round 15
</commit_message>
<xml_diff>
--- a/leagueStats/leagueStats_base_XGB.xlsx
+++ b/leagueStats/leagueStats_base_XGB.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O130"/>
+  <dimension ref="A1:O139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -532,10 +532,10 @@
         <v>0.34</v>
       </c>
       <c r="H2" t="n">
-        <v>0.68</v>
+        <v>0.59</v>
       </c>
       <c r="I2" t="n">
-        <v>0.24</v>
+        <v>0.29</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
@@ -544,13 +544,13 @@
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>0.21</v>
+        <v>0.12</v>
       </c>
       <c r="M2" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="N2" t="n">
-        <v>0.3</v>
+        <v>0.17</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
@@ -583,28 +583,28 @@
         <v>2.01</v>
       </c>
       <c r="H3" t="n">
-        <v>1.88</v>
+        <v>2.22</v>
       </c>
       <c r="I3" t="n">
-        <v>2.01</v>
+        <v>2.28</v>
       </c>
       <c r="J3" t="n">
         <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.47</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>0.27</v>
       </c>
       <c r="N3" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.74</v>
       </c>
       <c r="O3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -634,10 +634,10 @@
         <v>0.99</v>
       </c>
       <c r="H4" t="n">
-        <v>2.1</v>
+        <v>2.04</v>
       </c>
       <c r="I4" t="n">
-        <v>0.96</v>
+        <v>0.91</v>
       </c>
       <c r="J4" t="n">
         <v>0</v>
@@ -646,13 +646,13 @@
         <v>1</v>
       </c>
       <c r="L4" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.13</v>
       </c>
       <c r="M4" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
       <c r="N4" t="n">
-        <v>0.1</v>
+        <v>0.21</v>
       </c>
       <c r="O4" t="n">
         <v>3</v>
@@ -685,10 +685,10 @@
         <v>0.75</v>
       </c>
       <c r="H5" t="n">
-        <v>1.18</v>
+        <v>1.21</v>
       </c>
       <c r="I5" t="n">
-        <v>0.62</v>
+        <v>0.73</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
@@ -697,13 +697,13 @@
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>0.67</v>
+        <v>0.64</v>
       </c>
       <c r="M5" t="n">
-        <v>0.13</v>
+        <v>0.02</v>
       </c>
       <c r="N5" t="n">
-        <v>0.8</v>
+        <v>0.66</v>
       </c>
       <c r="O5" t="n">
         <v>2</v>
@@ -736,10 +736,10 @@
         <v>0.99</v>
       </c>
       <c r="H6" t="n">
-        <v>2.96</v>
+        <v>3.13</v>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>0.92</v>
       </c>
       <c r="J6" t="n">
         <v>1</v>
@@ -748,13 +748,13 @@
         <v>1</v>
       </c>
       <c r="L6" t="n">
-        <v>0.38</v>
+        <v>0.21</v>
       </c>
       <c r="M6" t="n">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="N6" t="n">
-        <v>0.39</v>
+        <v>0.28</v>
       </c>
       <c r="O6" t="n">
         <v>0</v>
@@ -787,7 +787,7 @@
         <v>0.96</v>
       </c>
       <c r="H7" t="n">
-        <v>1.14</v>
+        <v>1.19</v>
       </c>
       <c r="I7" t="n">
         <v>1.33</v>
@@ -799,13 +799,13 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="M7" t="n">
         <v>0.37</v>
       </c>
       <c r="N7" t="n">
-        <v>0.52</v>
+        <v>0.57</v>
       </c>
       <c r="O7" t="n">
         <v>0</v>
@@ -838,10 +838,10 @@
         <v>0.97</v>
       </c>
       <c r="H8" t="n">
-        <v>1.57</v>
+        <v>1.44</v>
       </c>
       <c r="I8" t="n">
-        <v>0.96</v>
+        <v>1.08</v>
       </c>
       <c r="J8" t="n">
         <v>1</v>
@@ -850,13 +850,13 @@
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>0.28</v>
+        <v>0.41</v>
       </c>
       <c r="M8" t="n">
-        <v>0.01</v>
+        <v>0.11</v>
       </c>
       <c r="N8" t="n">
-        <v>0.29</v>
+        <v>0.52</v>
       </c>
       <c r="O8" t="n">
         <v>2</v>
@@ -889,10 +889,10 @@
         <v>0.62</v>
       </c>
       <c r="H9" t="n">
-        <v>1.81</v>
+        <v>2</v>
       </c>
       <c r="I9" t="n">
-        <v>0.64</v>
+        <v>0.65</v>
       </c>
       <c r="J9" t="n">
         <v>1</v>
@@ -901,13 +901,13 @@
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>0.58</v>
+        <v>0.39</v>
       </c>
       <c r="M9" t="n">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="N9" t="n">
-        <v>0.6</v>
+        <v>0.42</v>
       </c>
       <c r="O9" t="n">
         <v>3</v>
@@ -940,10 +940,10 @@
         <v>0.17</v>
       </c>
       <c r="H10" t="n">
-        <v>1.16</v>
+        <v>0.98</v>
       </c>
       <c r="I10" t="n">
-        <v>0.21</v>
+        <v>0.16</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
@@ -952,13 +952,13 @@
         <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>0.06</v>
+        <v>0.24</v>
       </c>
       <c r="M10" t="n">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
       <c r="N10" t="n">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="O10" t="n">
         <v>3</v>
@@ -991,10 +991,10 @@
         <v>1.76</v>
       </c>
       <c r="H11" t="n">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>2.3</v>
+        <v>2.54</v>
       </c>
       <c r="J11" t="n">
         <v>0</v>
@@ -1003,13 +1003,13 @@
         <v>1</v>
       </c>
       <c r="L11" t="n">
-        <v>0.6</v>
+        <v>0.58</v>
       </c>
       <c r="M11" t="n">
-        <v>0.54</v>
+        <v>0.78</v>
       </c>
       <c r="N11" t="n">
-        <v>1.14</v>
+        <v>1.36</v>
       </c>
       <c r="O11" t="n">
         <v>3</v>
@@ -1042,7 +1042,7 @@
         <v>0.27</v>
       </c>
       <c r="H12" t="n">
-        <v>1.94</v>
+        <v>2.07</v>
       </c>
       <c r="I12" t="n">
         <v>0.32</v>
@@ -1054,13 +1054,13 @@
         <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>0.48</v>
+        <v>0.35</v>
       </c>
       <c r="M12" t="n">
         <v>0.05</v>
       </c>
       <c r="N12" t="n">
-        <v>0.53</v>
+        <v>0.4</v>
       </c>
       <c r="O12" t="n">
         <v>1</v>
@@ -1093,10 +1093,10 @@
         <v>0.6899999999999999</v>
       </c>
       <c r="H13" t="n">
-        <v>0.57</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="I13" t="n">
-        <v>0.45</v>
+        <v>0.54</v>
       </c>
       <c r="J13" t="n">
         <v>0</v>
@@ -1105,13 +1105,13 @@
         <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="M13" t="n">
-        <v>0.24</v>
+        <v>0.15</v>
       </c>
       <c r="N13" t="n">
-        <v>0.37</v>
+        <v>0.27</v>
       </c>
       <c r="O13" t="n">
         <v>1</v>
@@ -1144,10 +1144,10 @@
         <v>1.96</v>
       </c>
       <c r="H14" t="n">
-        <v>1.66</v>
+        <v>1.62</v>
       </c>
       <c r="I14" t="n">
-        <v>1.89</v>
+        <v>1.97</v>
       </c>
       <c r="J14" t="n">
         <v>0</v>
@@ -1156,13 +1156,13 @@
         <v>1</v>
       </c>
       <c r="L14" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.11</v>
       </c>
       <c r="M14" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.01</v>
       </c>
       <c r="N14" t="n">
-        <v>0.14</v>
+        <v>0.12</v>
       </c>
       <c r="O14" t="n">
         <v>2</v>
@@ -1195,10 +1195,10 @@
         <v>1.36</v>
       </c>
       <c r="H15" t="n">
-        <v>0.65</v>
+        <v>0.73</v>
       </c>
       <c r="I15" t="n">
-        <v>1.28</v>
+        <v>1.38</v>
       </c>
       <c r="J15" t="n">
         <v>0</v>
@@ -1207,13 +1207,13 @@
         <v>0</v>
       </c>
       <c r="L15" t="n">
-        <v>0.2</v>
+        <v>0.12</v>
       </c>
       <c r="M15" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
       <c r="N15" t="n">
-        <v>0.28</v>
+        <v>0.14</v>
       </c>
       <c r="O15" t="n">
         <v>3</v>
@@ -1246,10 +1246,10 @@
         <v>0.63</v>
       </c>
       <c r="H16" t="n">
-        <v>1.22</v>
+        <v>1.02</v>
       </c>
       <c r="I16" t="n">
-        <v>0.48</v>
+        <v>0.6</v>
       </c>
       <c r="J16" t="n">
         <v>0</v>
@@ -1258,13 +1258,13 @@
         <v>0</v>
       </c>
       <c r="L16" t="n">
-        <v>0.32</v>
+        <v>0.12</v>
       </c>
       <c r="M16" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N16" t="n">
         <v>0.15</v>
-      </c>
-      <c r="N16" t="n">
-        <v>0.47</v>
       </c>
       <c r="O16" t="n">
         <v>0</v>
@@ -1297,10 +1297,10 @@
         <v>0.64</v>
       </c>
       <c r="H17" t="n">
-        <v>2.03</v>
+        <v>1.99</v>
       </c>
       <c r="I17" t="n">
-        <v>0.42</v>
+        <v>0.36</v>
       </c>
       <c r="J17" t="n">
         <v>1</v>
@@ -1309,13 +1309,13 @@
         <v>0</v>
       </c>
       <c r="L17" t="n">
-        <v>0.43</v>
+        <v>0.47</v>
       </c>
       <c r="M17" t="n">
-        <v>0.22</v>
+        <v>0.28</v>
       </c>
       <c r="N17" t="n">
-        <v>0.65</v>
+        <v>0.75</v>
       </c>
       <c r="O17" t="n">
         <v>2</v>
@@ -1348,10 +1348,10 @@
         <v>2.94</v>
       </c>
       <c r="H18" t="n">
-        <v>2.17</v>
+        <v>2.26</v>
       </c>
       <c r="I18" t="n">
-        <v>2.66</v>
+        <v>2.61</v>
       </c>
       <c r="J18" t="n">
         <v>1</v>
@@ -1360,13 +1360,13 @@
         <v>1</v>
       </c>
       <c r="L18" t="n">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="M18" t="n">
-        <v>0.28</v>
+        <v>0.33</v>
       </c>
       <c r="N18" t="n">
-        <v>0.29</v>
+        <v>0.43</v>
       </c>
       <c r="O18" t="n">
         <v>1</v>
@@ -1399,10 +1399,10 @@
         <v>3.26</v>
       </c>
       <c r="H19" t="n">
-        <v>1.44</v>
+        <v>1.39</v>
       </c>
       <c r="I19" t="n">
-        <v>3.36</v>
+        <v>3.38</v>
       </c>
       <c r="J19" t="n">
         <v>0</v>
@@ -1411,13 +1411,13 @@
         <v>1</v>
       </c>
       <c r="L19" t="n">
-        <v>1.16</v>
+        <v>1.21</v>
       </c>
       <c r="M19" t="n">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="N19" t="n">
-        <v>1.26</v>
+        <v>1.33</v>
       </c>
       <c r="O19" t="n">
         <v>2</v>
@@ -1450,25 +1450,25 @@
         <v>1.53</v>
       </c>
       <c r="H20" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.97</v>
       </c>
       <c r="I20" t="n">
-        <v>2.09</v>
+        <v>1.74</v>
       </c>
       <c r="J20" t="n">
         <v>0</v>
       </c>
       <c r="K20" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L20" t="n">
-        <v>0.13</v>
+        <v>0.16</v>
       </c>
       <c r="M20" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.21</v>
       </c>
       <c r="N20" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.38</v>
       </c>
       <c r="O20" t="n">
         <v>2</v>
@@ -1501,10 +1501,10 @@
         <v>1.23</v>
       </c>
       <c r="H21" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.68</v>
       </c>
       <c r="I21" t="n">
-        <v>1.29</v>
+        <v>1.3</v>
       </c>
       <c r="J21" t="n">
         <v>0</v>
@@ -1513,13 +1513,13 @@
         <v>1</v>
       </c>
       <c r="L21" t="n">
-        <v>0.29</v>
+        <v>0.16</v>
       </c>
       <c r="M21" t="n">
-        <v>0.06</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="N21" t="n">
-        <v>0.35</v>
+        <v>0.23</v>
       </c>
       <c r="O21" t="n">
         <v>2</v>
@@ -1552,10 +1552,10 @@
         <v>1.37</v>
       </c>
       <c r="H22" t="n">
-        <v>2.45</v>
+        <v>2.17</v>
       </c>
       <c r="I22" t="n">
-        <v>0.95</v>
+        <v>0.99</v>
       </c>
       <c r="J22" t="n">
         <v>1</v>
@@ -1564,13 +1564,13 @@
         <v>0</v>
       </c>
       <c r="L22" t="n">
-        <v>1.14</v>
+        <v>0.86</v>
       </c>
       <c r="M22" t="n">
-        <v>0.42</v>
+        <v>0.38</v>
       </c>
       <c r="N22" t="n">
-        <v>1.55</v>
+        <v>1.24</v>
       </c>
       <c r="O22" t="n">
         <v>3</v>
@@ -1603,10 +1603,10 @@
         <v>1.1</v>
       </c>
       <c r="H23" t="n">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="I23" t="n">
-        <v>1.34</v>
+        <v>1.53</v>
       </c>
       <c r="J23" t="n">
         <v>0</v>
@@ -1615,13 +1615,13 @@
         <v>1</v>
       </c>
       <c r="L23" t="n">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="M23" t="n">
-        <v>0.24</v>
+        <v>0.43</v>
       </c>
       <c r="N23" t="n">
-        <v>0.28</v>
+        <v>0.49</v>
       </c>
       <c r="O23" t="n">
         <v>0</v>
@@ -1654,10 +1654,10 @@
         <v>0.97</v>
       </c>
       <c r="H24" t="n">
-        <v>1.62</v>
+        <v>1.67</v>
       </c>
       <c r="I24" t="n">
-        <v>0.71</v>
+        <v>0.76</v>
       </c>
       <c r="J24" t="n">
         <v>1</v>
@@ -1666,10 +1666,10 @@
         <v>1</v>
       </c>
       <c r="L24" t="n">
-        <v>0.26</v>
+        <v>0.31</v>
       </c>
       <c r="M24" t="n">
-        <v>0.26</v>
+        <v>0.21</v>
       </c>
       <c r="N24" t="n">
         <v>0.52</v>
@@ -1705,28 +1705,28 @@
         <v>1.29</v>
       </c>
       <c r="H25" t="n">
-        <v>1.63</v>
+        <v>1.65</v>
       </c>
       <c r="I25" t="n">
-        <v>1.37</v>
+        <v>1.29</v>
       </c>
       <c r="J25" t="n">
         <v>1</v>
       </c>
       <c r="K25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25" t="n">
-        <v>0.44</v>
+        <v>0.42</v>
       </c>
       <c r="M25" t="n">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="N25" t="n">
-        <v>0.53</v>
+        <v>0.42</v>
       </c>
       <c r="O25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26">
@@ -1756,28 +1756,28 @@
         <v>1.88</v>
       </c>
       <c r="H26" t="n">
-        <v>1.64</v>
+        <v>1.52</v>
       </c>
       <c r="I26" t="n">
-        <v>2.48</v>
+        <v>2.11</v>
       </c>
       <c r="J26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K26" t="n">
         <v>0</v>
       </c>
       <c r="L26" t="n">
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="M26" t="n">
-        <v>0.6</v>
+        <v>0.23</v>
       </c>
       <c r="N26" t="n">
-        <v>0.68</v>
+        <v>0.43</v>
       </c>
       <c r="O26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -1807,10 +1807,10 @@
         <v>1.76</v>
       </c>
       <c r="H27" t="n">
-        <v>1.92</v>
+        <v>2.39</v>
       </c>
       <c r="I27" t="n">
-        <v>1.65</v>
+        <v>1.77</v>
       </c>
       <c r="J27" t="n">
         <v>0</v>
@@ -1819,13 +1819,13 @@
         <v>1</v>
       </c>
       <c r="L27" t="n">
-        <v>0.27</v>
+        <v>0.2</v>
       </c>
       <c r="M27" t="n">
-        <v>0.11</v>
+        <v>0.01</v>
       </c>
       <c r="N27" t="n">
-        <v>0.37</v>
+        <v>0.21</v>
       </c>
       <c r="O27" t="n">
         <v>2</v>
@@ -1858,10 +1858,10 @@
         <v>0.3</v>
       </c>
       <c r="H28" t="n">
-        <v>2.5</v>
+        <v>2.37</v>
       </c>
       <c r="I28" t="n">
-        <v>0.38</v>
+        <v>0.35</v>
       </c>
       <c r="J28" t="n">
         <v>1</v>
@@ -1870,13 +1870,13 @@
         <v>0</v>
       </c>
       <c r="L28" t="n">
-        <v>0.4</v>
+        <v>0.27</v>
       </c>
       <c r="M28" t="n">
-        <v>0.08</v>
+        <v>0.05</v>
       </c>
       <c r="N28" t="n">
-        <v>0.49</v>
+        <v>0.31</v>
       </c>
       <c r="O28" t="n">
         <v>3</v>
@@ -1909,10 +1909,10 @@
         <v>1.54</v>
       </c>
       <c r="H29" t="n">
-        <v>1.14</v>
+        <v>1.13</v>
       </c>
       <c r="I29" t="n">
-        <v>1.4</v>
+        <v>1.25</v>
       </c>
       <c r="J29" t="n">
         <v>0</v>
@@ -1921,13 +1921,13 @@
         <v>1</v>
       </c>
       <c r="L29" t="n">
-        <v>0.36</v>
+        <v>0.37</v>
       </c>
       <c r="M29" t="n">
-        <v>0.14</v>
+        <v>0.29</v>
       </c>
       <c r="N29" t="n">
-        <v>0.5</v>
+        <v>0.66</v>
       </c>
       <c r="O29" t="n">
         <v>1</v>
@@ -1960,10 +1960,10 @@
         <v>0.33</v>
       </c>
       <c r="H30" t="n">
-        <v>0.72</v>
+        <v>0.7</v>
       </c>
       <c r="I30" t="n">
-        <v>0.68</v>
+        <v>0.57</v>
       </c>
       <c r="J30" t="n">
         <v>0</v>
@@ -1972,13 +1972,13 @@
         <v>0</v>
       </c>
       <c r="L30" t="n">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
       <c r="M30" t="n">
-        <v>0.35</v>
+        <v>0.24</v>
       </c>
       <c r="N30" t="n">
-        <v>0.57</v>
+        <v>0.44</v>
       </c>
       <c r="O30" t="n">
         <v>0</v>
@@ -2011,10 +2011,10 @@
         <v>1.68</v>
       </c>
       <c r="H31" t="n">
-        <v>1.34</v>
+        <v>1.3</v>
       </c>
       <c r="I31" t="n">
-        <v>2.11</v>
+        <v>1.85</v>
       </c>
       <c r="J31" t="n">
         <v>0</v>
@@ -2023,13 +2023,13 @@
         <v>1</v>
       </c>
       <c r="L31" t="n">
-        <v>0.36</v>
+        <v>0.32</v>
       </c>
       <c r="M31" t="n">
-        <v>0.43</v>
+        <v>0.17</v>
       </c>
       <c r="N31" t="n">
-        <v>0.79</v>
+        <v>0.49</v>
       </c>
       <c r="O31" t="n">
         <v>2</v>
@@ -2062,10 +2062,10 @@
         <v>1.2</v>
       </c>
       <c r="H32" t="n">
-        <v>0.96</v>
+        <v>1.03</v>
       </c>
       <c r="I32" t="n">
-        <v>1.34</v>
+        <v>1.12</v>
       </c>
       <c r="J32" t="n">
         <v>0</v>
@@ -2074,13 +2074,13 @@
         <v>0</v>
       </c>
       <c r="L32" t="n">
-        <v>0.21</v>
+        <v>0.14</v>
       </c>
       <c r="M32" t="n">
-        <v>0.14</v>
+        <v>0.08</v>
       </c>
       <c r="N32" t="n">
-        <v>0.34</v>
+        <v>0.22</v>
       </c>
       <c r="O32" t="n">
         <v>4</v>
@@ -2113,10 +2113,10 @@
         <v>0.89</v>
       </c>
       <c r="H33" t="n">
-        <v>0.34</v>
+        <v>0.54</v>
       </c>
       <c r="I33" t="n">
-        <v>0.85</v>
+        <v>1.16</v>
       </c>
       <c r="J33" t="n">
         <v>0</v>
@@ -2125,13 +2125,13 @@
         <v>0</v>
       </c>
       <c r="L33" t="n">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="M33" t="n">
-        <v>0.04</v>
+        <v>0.27</v>
       </c>
       <c r="N33" t="n">
-        <v>0.19</v>
+        <v>0.32</v>
       </c>
       <c r="O33" t="n">
         <v>0</v>
@@ -2164,7 +2164,7 @@
         <v>0.25</v>
       </c>
       <c r="H34" t="n">
-        <v>2.37</v>
+        <v>2.52</v>
       </c>
       <c r="I34" t="n">
         <v>0.23</v>
@@ -2176,13 +2176,13 @@
         <v>0</v>
       </c>
       <c r="L34" t="n">
-        <v>0.12</v>
+        <v>0.27</v>
       </c>
       <c r="M34" t="n">
         <v>0.02</v>
       </c>
       <c r="N34" t="n">
-        <v>0.15</v>
+        <v>0.29</v>
       </c>
       <c r="O34" t="n">
         <v>2</v>
@@ -2215,10 +2215,10 @@
         <v>2.06</v>
       </c>
       <c r="H35" t="n">
-        <v>1.43</v>
+        <v>1.68</v>
       </c>
       <c r="I35" t="n">
-        <v>1.79</v>
+        <v>1.65</v>
       </c>
       <c r="J35" t="n">
         <v>0</v>
@@ -2227,13 +2227,13 @@
         <v>1</v>
       </c>
       <c r="L35" t="n">
-        <v>0.22</v>
+        <v>0.03</v>
       </c>
       <c r="M35" t="n">
-        <v>0.27</v>
+        <v>0.41</v>
       </c>
       <c r="N35" t="n">
-        <v>0.48</v>
+        <v>0.44</v>
       </c>
       <c r="O35" t="n">
         <v>4</v>
@@ -2266,28 +2266,28 @@
         <v>1.93</v>
       </c>
       <c r="H36" t="n">
-        <v>1.42</v>
+        <v>1.3</v>
       </c>
       <c r="I36" t="n">
-        <v>2.17</v>
+        <v>1.9</v>
       </c>
       <c r="J36" t="n">
         <v>0</v>
       </c>
       <c r="K36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L36" t="n">
-        <v>0.4</v>
+        <v>0.28</v>
       </c>
       <c r="M36" t="n">
-        <v>0.24</v>
+        <v>0.03</v>
       </c>
       <c r="N36" t="n">
-        <v>0.64</v>
+        <v>0.31</v>
       </c>
       <c r="O36" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37">
@@ -2317,28 +2317,28 @@
         <v>2.22</v>
       </c>
       <c r="H37" t="n">
-        <v>1.49</v>
+        <v>1.42</v>
       </c>
       <c r="I37" t="n">
-        <v>2</v>
+        <v>2.16</v>
       </c>
       <c r="J37" t="n">
         <v>0</v>
       </c>
       <c r="K37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L37" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="N37" t="n">
         <v>0.24</v>
       </c>
-      <c r="M37" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="N37" t="n">
-        <v>0.46</v>
-      </c>
       <c r="O37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -2368,10 +2368,10 @@
         <v>1.66</v>
       </c>
       <c r="H38" t="n">
-        <v>0.18</v>
+        <v>0.21</v>
       </c>
       <c r="I38" t="n">
-        <v>1.79</v>
+        <v>2</v>
       </c>
       <c r="J38" t="n">
         <v>0</v>
@@ -2380,13 +2380,13 @@
         <v>0</v>
       </c>
       <c r="L38" t="n">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="M38" t="n">
-        <v>0.13</v>
+        <v>0.34</v>
       </c>
       <c r="N38" t="n">
-        <v>0.19</v>
+        <v>0.37</v>
       </c>
       <c r="O38" t="n">
         <v>2</v>
@@ -2419,10 +2419,10 @@
         <v>1.6</v>
       </c>
       <c r="H39" t="n">
-        <v>0.37</v>
+        <v>0.43</v>
       </c>
       <c r="I39" t="n">
-        <v>1.3</v>
+        <v>1.36</v>
       </c>
       <c r="J39" t="n">
         <v>0</v>
@@ -2431,13 +2431,13 @@
         <v>0</v>
       </c>
       <c r="L39" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
       <c r="M39" t="n">
-        <v>0.3</v>
+        <v>0.24</v>
       </c>
       <c r="N39" t="n">
-        <v>0.38</v>
+        <v>0.25</v>
       </c>
       <c r="O39" t="n">
         <v>0</v>
@@ -2470,25 +2470,25 @@
         <v>0.83</v>
       </c>
       <c r="H40" t="n">
-        <v>1.3</v>
+        <v>1.41</v>
       </c>
       <c r="I40" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0</v>
+      </c>
+      <c r="L40" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="M40" t="n">
         <v>0.39</v>
       </c>
-      <c r="J40" t="n">
-        <v>0</v>
-      </c>
-      <c r="K40" t="n">
-        <v>0</v>
-      </c>
-      <c r="L40" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="M40" t="n">
-        <v>0.44</v>
-      </c>
       <c r="N40" t="n">
-        <v>0.51</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="O40" t="n">
         <v>3</v>
@@ -2521,25 +2521,25 @@
         <v>2.74</v>
       </c>
       <c r="H41" t="n">
-        <v>1.14</v>
+        <v>0.95</v>
       </c>
       <c r="I41" t="n">
-        <v>3.22</v>
+        <v>3.04</v>
       </c>
       <c r="J41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L41" t="n">
-        <v>0.34</v>
+        <v>0.15</v>
       </c>
       <c r="M41" t="n">
-        <v>0.48</v>
+        <v>0.3</v>
       </c>
       <c r="N41" t="n">
-        <v>0.82</v>
+        <v>0.45</v>
       </c>
       <c r="O41" t="n">
         <v>3</v>
@@ -2572,10 +2572,10 @@
         <v>0.85</v>
       </c>
       <c r="H42" t="n">
-        <v>2.43</v>
+        <v>2.24</v>
       </c>
       <c r="I42" t="n">
-        <v>0.75</v>
+        <v>0.74</v>
       </c>
       <c r="J42" t="n">
         <v>1</v>
@@ -2584,13 +2584,13 @@
         <v>0</v>
       </c>
       <c r="L42" t="n">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="M42" t="n">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="N42" t="n">
-        <v>0.19</v>
+        <v>0.21</v>
       </c>
       <c r="O42" t="n">
         <v>3</v>
@@ -2623,7 +2623,7 @@
         <v>2.29</v>
       </c>
       <c r="H43" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.61</v>
       </c>
       <c r="I43" t="n">
         <v>2.18</v>
@@ -2635,13 +2635,13 @@
         <v>1</v>
       </c>
       <c r="L43" t="n">
-        <v>0.06</v>
+        <v>0.11</v>
       </c>
       <c r="M43" t="n">
         <v>0.11</v>
       </c>
       <c r="N43" t="n">
-        <v>0.17</v>
+        <v>0.22</v>
       </c>
       <c r="O43" t="n">
         <v>4</v>
@@ -2674,10 +2674,10 @@
         <v>0.31</v>
       </c>
       <c r="H44" t="n">
-        <v>0.43</v>
+        <v>0.36</v>
       </c>
       <c r="I44" t="n">
-        <v>0.38</v>
+        <v>0.39</v>
       </c>
       <c r="J44" t="n">
         <v>0</v>
@@ -2686,13 +2686,13 @@
         <v>0</v>
       </c>
       <c r="L44" t="n">
-        <v>0.12</v>
+        <v>0.05</v>
       </c>
       <c r="M44" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="N44" t="n">
-        <v>0.19</v>
+        <v>0.14</v>
       </c>
       <c r="O44" t="n">
         <v>0</v>
@@ -2725,10 +2725,10 @@
         <v>2.11</v>
       </c>
       <c r="H45" t="n">
-        <v>1.21</v>
+        <v>1.46</v>
       </c>
       <c r="I45" t="n">
-        <v>2.15</v>
+        <v>2.03</v>
       </c>
       <c r="J45" t="n">
         <v>0</v>
@@ -2737,13 +2737,13 @@
         <v>0</v>
       </c>
       <c r="L45" t="n">
-        <v>0.3</v>
+        <v>0.05</v>
       </c>
       <c r="M45" t="n">
-        <v>0.04</v>
+        <v>0.08</v>
       </c>
       <c r="N45" t="n">
-        <v>0.34</v>
+        <v>0.13</v>
       </c>
       <c r="O45" t="n">
         <v>4</v>
@@ -2776,10 +2776,10 @@
         <v>0.5</v>
       </c>
       <c r="H46" t="n">
-        <v>1.69</v>
+        <v>1.63</v>
       </c>
       <c r="I46" t="n">
-        <v>0.84</v>
+        <v>0.7</v>
       </c>
       <c r="J46" t="n">
         <v>1</v>
@@ -2791,10 +2791,10 @@
         <v>0.03</v>
       </c>
       <c r="M46" t="n">
-        <v>0.34</v>
+        <v>0.2</v>
       </c>
       <c r="N46" t="n">
-        <v>0.37</v>
+        <v>0.23</v>
       </c>
       <c r="O46" t="n">
         <v>1</v>
@@ -2827,7 +2827,7 @@
         <v>1.05</v>
       </c>
       <c r="H47" t="n">
-        <v>2.64</v>
+        <v>3.02</v>
       </c>
       <c r="I47" t="n">
         <v>1.19</v>
@@ -2839,13 +2839,13 @@
         <v>0</v>
       </c>
       <c r="L47" t="n">
-        <v>0.14</v>
+        <v>0.24</v>
       </c>
       <c r="M47" t="n">
         <v>0.14</v>
       </c>
       <c r="N47" t="n">
-        <v>0.28</v>
+        <v>0.38</v>
       </c>
       <c r="O47" t="n">
         <v>1</v>
@@ -2878,10 +2878,10 @@
         <v>1.7</v>
       </c>
       <c r="H48" t="n">
-        <v>0.9</v>
+        <v>1.2</v>
       </c>
       <c r="I48" t="n">
-        <v>1.65</v>
+        <v>1.94</v>
       </c>
       <c r="J48" t="n">
         <v>0</v>
@@ -2890,13 +2890,13 @@
         <v>0</v>
       </c>
       <c r="L48" t="n">
-        <v>0.17</v>
+        <v>0.47</v>
       </c>
       <c r="M48" t="n">
-        <v>0.05</v>
+        <v>0.24</v>
       </c>
       <c r="N48" t="n">
-        <v>0.21</v>
+        <v>0.71</v>
       </c>
       <c r="O48" t="n">
         <v>3</v>
@@ -2929,10 +2929,10 @@
         <v>0.76</v>
       </c>
       <c r="H49" t="n">
-        <v>0.49</v>
+        <v>0.44</v>
       </c>
       <c r="I49" t="n">
-        <v>0.98</v>
+        <v>1.04</v>
       </c>
       <c r="J49" t="n">
         <v>0</v>
@@ -2941,13 +2941,13 @@
         <v>0</v>
       </c>
       <c r="L49" t="n">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="M49" t="n">
-        <v>0.22</v>
+        <v>0.28</v>
       </c>
       <c r="N49" t="n">
-        <v>0.32</v>
+        <v>0.43</v>
       </c>
       <c r="O49" t="n">
         <v>3</v>
@@ -2980,10 +2980,10 @@
         <v>0.73</v>
       </c>
       <c r="H50" t="n">
-        <v>2.54</v>
+        <v>2.4</v>
       </c>
       <c r="I50" t="n">
-        <v>1.09</v>
+        <v>0.79</v>
       </c>
       <c r="J50" t="n">
         <v>1</v>
@@ -2992,13 +2992,13 @@
         <v>0</v>
       </c>
       <c r="L50" t="n">
-        <v>0.64</v>
+        <v>0.5</v>
       </c>
       <c r="M50" t="n">
-        <v>0.36</v>
+        <v>0.06</v>
       </c>
       <c r="N50" t="n">
-        <v>1</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="O50" t="n">
         <v>2</v>
@@ -3031,10 +3031,10 @@
         <v>1.07</v>
       </c>
       <c r="H51" t="n">
-        <v>1.34</v>
+        <v>1.39</v>
       </c>
       <c r="I51" t="n">
-        <v>0.84</v>
+        <v>0.98</v>
       </c>
       <c r="J51" t="n">
         <v>1</v>
@@ -3043,13 +3043,13 @@
         <v>0</v>
       </c>
       <c r="L51" t="n">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="M51" t="n">
-        <v>0.23</v>
+        <v>0.09</v>
       </c>
       <c r="N51" t="n">
-        <v>0.47</v>
+        <v>0.29</v>
       </c>
       <c r="O51" t="n">
         <v>4</v>
@@ -3082,10 +3082,10 @@
         <v>0.49</v>
       </c>
       <c r="H52" t="n">
-        <v>1.82</v>
+        <v>1.87</v>
       </c>
       <c r="I52" t="n">
-        <v>0.6</v>
+        <v>0.67</v>
       </c>
       <c r="J52" t="n">
         <v>0</v>
@@ -3094,13 +3094,13 @@
         <v>0</v>
       </c>
       <c r="L52" t="n">
-        <v>0.11</v>
+        <v>0.16</v>
       </c>
       <c r="M52" t="n">
-        <v>0.11</v>
+        <v>0.18</v>
       </c>
       <c r="N52" t="n">
-        <v>0.22</v>
+        <v>0.34</v>
       </c>
       <c r="O52" t="n">
         <v>3</v>
@@ -3133,10 +3133,10 @@
         <v>2</v>
       </c>
       <c r="H53" t="n">
-        <v>0.22</v>
+        <v>0.23</v>
       </c>
       <c r="I53" t="n">
-        <v>1.81</v>
+        <v>1.92</v>
       </c>
       <c r="J53" t="n">
         <v>0</v>
@@ -3145,13 +3145,13 @@
         <v>0</v>
       </c>
       <c r="L53" t="n">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="M53" t="n">
-        <v>0.19</v>
+        <v>0.08</v>
       </c>
       <c r="N53" t="n">
-        <v>0.31</v>
+        <v>0.21</v>
       </c>
       <c r="O53" t="n">
         <v>2</v>
@@ -3184,28 +3184,28 @@
         <v>2.6</v>
       </c>
       <c r="H54" t="n">
-        <v>0.41</v>
+        <v>0.36</v>
       </c>
       <c r="I54" t="n">
-        <v>2.36</v>
+        <v>2.42</v>
       </c>
       <c r="J54" t="n">
         <v>0</v>
       </c>
       <c r="K54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L54" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
       <c r="M54" t="n">
-        <v>0.24</v>
+        <v>0.18</v>
       </c>
       <c r="N54" t="n">
-        <v>0.27</v>
+        <v>0.25</v>
       </c>
       <c r="O54" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55">
@@ -3235,10 +3235,10 @@
         <v>2.22</v>
       </c>
       <c r="H55" t="n">
-        <v>0.89</v>
+        <v>0.76</v>
       </c>
       <c r="I55" t="n">
-        <v>2.22</v>
+        <v>2.27</v>
       </c>
       <c r="J55" t="n">
         <v>0</v>
@@ -3247,13 +3247,13 @@
         <v>0</v>
       </c>
       <c r="L55" t="n">
-        <v>0.12</v>
+        <v>0.01</v>
       </c>
       <c r="M55" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="N55" t="n">
-        <v>0.13</v>
+        <v>0.06</v>
       </c>
       <c r="O55" t="n">
         <v>5</v>
@@ -3286,10 +3286,10 @@
         <v>1.14</v>
       </c>
       <c r="H56" t="n">
-        <v>1.87</v>
+        <v>2.04</v>
       </c>
       <c r="I56" t="n">
-        <v>1.25</v>
+        <v>1.07</v>
       </c>
       <c r="J56" t="n">
         <v>1</v>
@@ -3298,13 +3298,13 @@
         <v>1</v>
       </c>
       <c r="L56" t="n">
-        <v>0.38</v>
+        <v>0.21</v>
       </c>
       <c r="M56" t="n">
-        <v>0.11</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="N56" t="n">
-        <v>0.49</v>
+        <v>0.28</v>
       </c>
       <c r="O56" t="n">
         <v>3</v>
@@ -3337,25 +3337,25 @@
         <v>0.68</v>
       </c>
       <c r="H57" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="J57" t="n">
+        <v>0</v>
+      </c>
+      <c r="K57" t="n">
+        <v>0</v>
+      </c>
+      <c r="L57" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="M57" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="N57" t="n">
         <v>0.45</v>
-      </c>
-      <c r="I57" t="n">
-        <v>0.76</v>
-      </c>
-      <c r="J57" t="n">
-        <v>0</v>
-      </c>
-      <c r="K57" t="n">
-        <v>0</v>
-      </c>
-      <c r="L57" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="M57" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="N57" t="n">
-        <v>0.17</v>
       </c>
       <c r="O57" t="n">
         <v>0</v>
@@ -3388,10 +3388,10 @@
         <v>0.3</v>
       </c>
       <c r="H58" t="n">
-        <v>1.36</v>
+        <v>1.53</v>
       </c>
       <c r="I58" t="n">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
       <c r="J58" t="n">
         <v>0</v>
@@ -3400,13 +3400,13 @@
         <v>0</v>
       </c>
       <c r="L58" t="n">
-        <v>0.19</v>
+        <v>0.36</v>
       </c>
       <c r="M58" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="N58" t="n">
-        <v>0.26</v>
+        <v>0.44</v>
       </c>
       <c r="O58" t="n">
         <v>2</v>
@@ -3439,10 +3439,10 @@
         <v>1.8</v>
       </c>
       <c r="H59" t="n">
-        <v>1.64</v>
+        <v>1.73</v>
       </c>
       <c r="I59" t="n">
-        <v>1.91</v>
+        <v>1.93</v>
       </c>
       <c r="J59" t="n">
         <v>0</v>
@@ -3451,13 +3451,13 @@
         <v>0</v>
       </c>
       <c r="L59" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="M59" t="n">
-        <v>0.11</v>
+        <v>0.13</v>
       </c>
       <c r="N59" t="n">
-        <v>0.15</v>
+        <v>0.19</v>
       </c>
       <c r="O59" t="n">
         <v>3</v>
@@ -3490,10 +3490,10 @@
         <v>2.12</v>
       </c>
       <c r="H60" t="n">
-        <v>0.78</v>
+        <v>0.79</v>
       </c>
       <c r="I60" t="n">
-        <v>2.32</v>
+        <v>2.27</v>
       </c>
       <c r="J60" t="n">
         <v>0</v>
@@ -3502,13 +3502,13 @@
         <v>1</v>
       </c>
       <c r="L60" t="n">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="M60" t="n">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="N60" t="n">
-        <v>0.3</v>
+        <v>0.26</v>
       </c>
       <c r="O60" t="n">
         <v>4</v>
@@ -3541,10 +3541,10 @@
         <v>2.38</v>
       </c>
       <c r="H61" t="n">
-        <v>2.26</v>
+        <v>1.97</v>
       </c>
       <c r="I61" t="n">
-        <v>1.32</v>
+        <v>1.6</v>
       </c>
       <c r="J61" t="n">
         <v>1</v>
@@ -3553,13 +3553,13 @@
         <v>0</v>
       </c>
       <c r="L61" t="n">
-        <v>0.12</v>
+        <v>0.41</v>
       </c>
       <c r="M61" t="n">
-        <v>1.06</v>
+        <v>0.78</v>
       </c>
       <c r="N61" t="n">
-        <v>1.17</v>
+        <v>1.2</v>
       </c>
       <c r="O61" t="n">
         <v>4</v>
@@ -3592,10 +3592,10 @@
         <v>0.9</v>
       </c>
       <c r="H62" t="n">
-        <v>2.6</v>
+        <v>2.76</v>
       </c>
       <c r="I62" t="n">
-        <v>1.03</v>
+        <v>1</v>
       </c>
       <c r="J62" t="n">
         <v>0</v>
@@ -3604,13 +3604,13 @@
         <v>0</v>
       </c>
       <c r="L62" t="n">
-        <v>0.2</v>
+        <v>0.36</v>
       </c>
       <c r="M62" t="n">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="N62" t="n">
-        <v>0.32</v>
+        <v>0.46</v>
       </c>
       <c r="O62" t="n">
         <v>3</v>
@@ -3643,10 +3643,10 @@
         <v>0.37</v>
       </c>
       <c r="H63" t="n">
-        <v>1.69</v>
+        <v>2.07</v>
       </c>
       <c r="I63" t="n">
-        <v>0.59</v>
+        <v>0.51</v>
       </c>
       <c r="J63" t="n">
         <v>1</v>
@@ -3655,13 +3655,13 @@
         <v>0</v>
       </c>
       <c r="L63" t="n">
-        <v>0.22</v>
+        <v>0.16</v>
       </c>
       <c r="M63" t="n">
-        <v>0.22</v>
+        <v>0.14</v>
       </c>
       <c r="N63" t="n">
-        <v>0.44</v>
+        <v>0.3</v>
       </c>
       <c r="O63" t="n">
         <v>3</v>
@@ -3694,28 +3694,28 @@
         <v>0.73</v>
       </c>
       <c r="H64" t="n">
-        <v>4.45</v>
+        <v>4.02</v>
       </c>
       <c r="I64" t="n">
-        <v>0.49</v>
+        <v>0.48</v>
       </c>
       <c r="J64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K64" t="n">
         <v>0</v>
       </c>
       <c r="L64" t="n">
-        <v>0.78</v>
+        <v>0.35</v>
       </c>
       <c r="M64" t="n">
-        <v>0.24</v>
+        <v>0.25</v>
       </c>
       <c r="N64" t="n">
-        <v>1.02</v>
+        <v>0.6</v>
       </c>
       <c r="O64" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65">
@@ -3745,10 +3745,10 @@
         <v>1.61</v>
       </c>
       <c r="H65" t="n">
-        <v>2.49</v>
+        <v>2.68</v>
       </c>
       <c r="I65" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.96</v>
       </c>
       <c r="J65" t="n">
         <v>0</v>
@@ -3757,13 +3757,13 @@
         <v>1</v>
       </c>
       <c r="L65" t="n">
-        <v>0</v>
+        <v>0.19</v>
       </c>
       <c r="M65" t="n">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="N65" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.84</v>
       </c>
       <c r="O65" t="n">
         <v>4</v>
@@ -3796,10 +3796,10 @@
         <v>0.51</v>
       </c>
       <c r="H66" t="n">
-        <v>0.92</v>
+        <v>0.9</v>
       </c>
       <c r="I66" t="n">
-        <v>0.46</v>
+        <v>0.49</v>
       </c>
       <c r="J66" t="n">
         <v>0</v>
@@ -3808,13 +3808,13 @@
         <v>0</v>
       </c>
       <c r="L66" t="n">
+        <v>0</v>
+      </c>
+      <c r="M66" t="n">
         <v>0.02</v>
       </c>
-      <c r="M66" t="n">
-        <v>0.05</v>
-      </c>
       <c r="N66" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.03</v>
       </c>
       <c r="O66" t="n">
         <v>1</v>
@@ -3847,10 +3847,10 @@
         <v>0.77</v>
       </c>
       <c r="H67" t="n">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="I67" t="n">
-        <v>0.89</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="J67" t="n">
         <v>0</v>
@@ -3859,13 +3859,13 @@
         <v>0</v>
       </c>
       <c r="L67" t="n">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="M67" t="n">
-        <v>0.12</v>
+        <v>0.17</v>
       </c>
       <c r="N67" t="n">
-        <v>0.17</v>
+        <v>0.37</v>
       </c>
       <c r="O67" t="n">
         <v>0</v>
@@ -3898,28 +3898,28 @@
         <v>2.67</v>
       </c>
       <c r="H68" t="n">
-        <v>1.76</v>
+        <v>1.85</v>
       </c>
       <c r="I68" t="n">
-        <v>2.44</v>
+        <v>2.87</v>
       </c>
       <c r="J68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K68" t="n">
         <v>2</v>
       </c>
       <c r="L68" t="n">
-        <v>0.29</v>
+        <v>0.38</v>
       </c>
       <c r="M68" t="n">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="N68" t="n">
-        <v>0.52</v>
+        <v>0.58</v>
       </c>
       <c r="O68" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69">
@@ -3949,10 +3949,10 @@
         <v>1.12</v>
       </c>
       <c r="H69" t="n">
-        <v>2.38</v>
+        <v>2.78</v>
       </c>
       <c r="I69" t="n">
-        <v>1.16</v>
+        <v>1.14</v>
       </c>
       <c r="J69" t="n">
         <v>1</v>
@@ -3961,13 +3961,13 @@
         <v>1</v>
       </c>
       <c r="L69" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="M69" t="n">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="N69" t="n">
-        <v>0.14</v>
+        <v>0.32</v>
       </c>
       <c r="O69" t="n">
         <v>0</v>
@@ -4000,10 +4000,10 @@
         <v>0.55</v>
       </c>
       <c r="H70" t="n">
-        <v>2.07</v>
+        <v>2.17</v>
       </c>
       <c r="I70" t="n">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="J70" t="n">
         <v>1</v>
@@ -4012,13 +4012,13 @@
         <v>0</v>
       </c>
       <c r="L70" t="n">
-        <v>0.32</v>
+        <v>0.22</v>
       </c>
       <c r="M70" t="n">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="N70" t="n">
-        <v>0.47</v>
+        <v>0.42</v>
       </c>
       <c r="O70" t="n">
         <v>2</v>
@@ -4051,28 +4051,28 @@
         <v>1.07</v>
       </c>
       <c r="H71" t="n">
-        <v>0.76</v>
+        <v>0.54</v>
       </c>
       <c r="I71" t="n">
-        <v>1.09</v>
+        <v>1.13</v>
       </c>
       <c r="J71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K71" t="n">
         <v>0</v>
       </c>
       <c r="L71" t="n">
-        <v>0.36</v>
+        <v>0.58</v>
       </c>
       <c r="M71" t="n">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
       <c r="N71" t="n">
-        <v>0.38</v>
+        <v>0.64</v>
       </c>
       <c r="O71" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72">
@@ -4102,10 +4102,10 @@
         <v>0.48</v>
       </c>
       <c r="H72" t="n">
-        <v>1.34</v>
+        <v>1.23</v>
       </c>
       <c r="I72" t="n">
-        <v>0.83</v>
+        <v>0.68</v>
       </c>
       <c r="J72" t="n">
         <v>0</v>
@@ -4114,13 +4114,13 @@
         <v>0</v>
       </c>
       <c r="L72" t="n">
-        <v>0.04</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="M72" t="n">
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="N72" t="n">
-        <v>0.39</v>
+        <v>0.27</v>
       </c>
       <c r="O72" t="n">
         <v>2</v>
@@ -4153,10 +4153,10 @@
         <v>0.67</v>
       </c>
       <c r="H73" t="n">
-        <v>0.45</v>
+        <v>0.55</v>
       </c>
       <c r="I73" t="n">
-        <v>0.77</v>
+        <v>0.9</v>
       </c>
       <c r="J73" t="n">
         <v>0</v>
@@ -4165,13 +4165,13 @@
         <v>0</v>
       </c>
       <c r="L73" t="n">
-        <v>0.03</v>
+        <v>0.13</v>
       </c>
       <c r="M73" t="n">
-        <v>0.1</v>
+        <v>0.23</v>
       </c>
       <c r="N73" t="n">
-        <v>0.13</v>
+        <v>0.36</v>
       </c>
       <c r="O73" t="n">
         <v>4</v>
@@ -4204,10 +4204,10 @@
         <v>0.05</v>
       </c>
       <c r="H74" t="n">
-        <v>1.14</v>
+        <v>1.5</v>
       </c>
       <c r="I74" t="n">
-        <v>0.14</v>
+        <v>0.15</v>
       </c>
       <c r="J74" t="n">
         <v>0</v>
@@ -4216,13 +4216,13 @@
         <v>0</v>
       </c>
       <c r="L74" t="n">
-        <v>0.21</v>
+        <v>0.15</v>
       </c>
       <c r="M74" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="N74" t="n">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="O74" t="n">
         <v>1</v>
@@ -4255,10 +4255,10 @@
         <v>0.44</v>
       </c>
       <c r="H75" t="n">
-        <v>1.66</v>
+        <v>1.87</v>
       </c>
       <c r="I75" t="n">
-        <v>0.63</v>
+        <v>0.52</v>
       </c>
       <c r="J75" t="n">
         <v>1</v>
@@ -4267,13 +4267,13 @@
         <v>0</v>
       </c>
       <c r="L75" t="n">
-        <v>0.44</v>
+        <v>0.65</v>
       </c>
       <c r="M75" t="n">
-        <v>0.19</v>
+        <v>0.08</v>
       </c>
       <c r="N75" t="n">
-        <v>0.63</v>
+        <v>0.73</v>
       </c>
       <c r="O75" t="n">
         <v>0</v>
@@ -4306,10 +4306,10 @@
         <v>1.44</v>
       </c>
       <c r="H76" t="n">
-        <v>1.27</v>
+        <v>1.26</v>
       </c>
       <c r="I76" t="n">
-        <v>1.69</v>
+        <v>1.76</v>
       </c>
       <c r="J76" t="n">
         <v>0</v>
@@ -4318,13 +4318,13 @@
         <v>1</v>
       </c>
       <c r="L76" t="n">
-        <v>0.39</v>
+        <v>0.4</v>
       </c>
       <c r="M76" t="n">
-        <v>0.25</v>
+        <v>0.32</v>
       </c>
       <c r="N76" t="n">
-        <v>0.64</v>
+        <v>0.73</v>
       </c>
       <c r="O76" t="n">
         <v>4</v>
@@ -4357,10 +4357,10 @@
         <v>1.41</v>
       </c>
       <c r="H77" t="n">
-        <v>0.87</v>
+        <v>0.83</v>
       </c>
       <c r="I77" t="n">
-        <v>1.54</v>
+        <v>1.88</v>
       </c>
       <c r="J77" t="n">
         <v>0</v>
@@ -4369,13 +4369,13 @@
         <v>1</v>
       </c>
       <c r="L77" t="n">
-        <v>0.16</v>
+        <v>0.12</v>
       </c>
       <c r="M77" t="n">
-        <v>0.13</v>
+        <v>0.47</v>
       </c>
       <c r="N77" t="n">
-        <v>0.29</v>
+        <v>0.58</v>
       </c>
       <c r="O77" t="n">
         <v>0</v>
@@ -4408,28 +4408,28 @@
         <v>2.26</v>
       </c>
       <c r="H78" t="n">
-        <v>0.29</v>
+        <v>0.32</v>
       </c>
       <c r="I78" t="n">
-        <v>3.19</v>
+        <v>2.8</v>
       </c>
       <c r="J78" t="n">
         <v>0</v>
       </c>
       <c r="K78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L78" t="n">
-        <v>0.06</v>
+        <v>0.09</v>
       </c>
       <c r="M78" t="n">
-        <v>0.93</v>
+        <v>0.54</v>
       </c>
       <c r="N78" t="n">
-        <v>0.99</v>
+        <v>0.63</v>
       </c>
       <c r="O78" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79">
@@ -4459,10 +4459,10 @@
         <v>0.97</v>
       </c>
       <c r="H79" t="n">
-        <v>1.5</v>
+        <v>1.53</v>
       </c>
       <c r="I79" t="n">
-        <v>0.96</v>
+        <v>1.22</v>
       </c>
       <c r="J79" t="n">
         <v>0</v>
@@ -4471,13 +4471,13 @@
         <v>0</v>
       </c>
       <c r="L79" t="n">
-        <v>0.46</v>
+        <v>0.49</v>
       </c>
       <c r="M79" t="n">
-        <v>0.01</v>
+        <v>0.25</v>
       </c>
       <c r="N79" t="n">
-        <v>0.47</v>
+        <v>0.74</v>
       </c>
       <c r="O79" t="n">
         <v>1</v>
@@ -4510,10 +4510,10 @@
         <v>1.4</v>
       </c>
       <c r="H80" t="n">
-        <v>0.65</v>
+        <v>0.68</v>
       </c>
       <c r="I80" t="n">
-        <v>1.35</v>
+        <v>1.8</v>
       </c>
       <c r="J80" t="n">
         <v>0</v>
@@ -4522,13 +4522,13 @@
         <v>1</v>
       </c>
       <c r="L80" t="n">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="M80" t="n">
-        <v>0.05</v>
+        <v>0.4</v>
       </c>
       <c r="N80" t="n">
-        <v>0.2</v>
+        <v>0.53</v>
       </c>
       <c r="O80" t="n">
         <v>1</v>
@@ -4561,10 +4561,10 @@
         <v>1.39</v>
       </c>
       <c r="H81" t="n">
-        <v>1.24</v>
+        <v>0.97</v>
       </c>
       <c r="I81" t="n">
-        <v>0.74</v>
+        <v>0.8</v>
       </c>
       <c r="J81" t="n">
         <v>0</v>
@@ -4573,13 +4573,13 @@
         <v>0</v>
       </c>
       <c r="L81" t="n">
-        <v>0.31</v>
+        <v>0.04</v>
       </c>
       <c r="M81" t="n">
-        <v>0.65</v>
+        <v>0.59</v>
       </c>
       <c r="N81" t="n">
-        <v>0.96</v>
+        <v>0.63</v>
       </c>
       <c r="O81" t="n">
         <v>3</v>
@@ -4612,10 +4612,10 @@
         <v>1.48</v>
       </c>
       <c r="H82" t="n">
-        <v>0.66</v>
+        <v>0.67</v>
       </c>
       <c r="I82" t="n">
-        <v>1.14</v>
+        <v>1.22</v>
       </c>
       <c r="J82" t="n">
         <v>0</v>
@@ -4624,13 +4624,13 @@
         <v>0</v>
       </c>
       <c r="L82" t="n">
-        <v>0.64</v>
+        <v>0.63</v>
       </c>
       <c r="M82" t="n">
-        <v>0.34</v>
+        <v>0.26</v>
       </c>
       <c r="N82" t="n">
-        <v>0.98</v>
+        <v>0.9</v>
       </c>
       <c r="O82" t="n">
         <v>1</v>
@@ -4663,10 +4663,10 @@
         <v>0.43</v>
       </c>
       <c r="H83" t="n">
-        <v>0.78</v>
+        <v>0.93</v>
       </c>
       <c r="I83" t="n">
-        <v>0.47</v>
+        <v>0.42</v>
       </c>
       <c r="J83" t="n">
         <v>0</v>
@@ -4675,13 +4675,13 @@
         <v>0</v>
       </c>
       <c r="L83" t="n">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="M83" t="n">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
       <c r="N83" t="n">
-        <v>0.29</v>
+        <v>0.12</v>
       </c>
       <c r="O83" t="n">
         <v>2</v>
@@ -4714,10 +4714,10 @@
         <v>0.21</v>
       </c>
       <c r="H84" t="n">
-        <v>3.01</v>
+        <v>3.25</v>
       </c>
       <c r="I84" t="n">
-        <v>0.26</v>
+        <v>0.25</v>
       </c>
       <c r="J84" t="n">
         <v>1</v>
@@ -4726,13 +4726,13 @@
         <v>0</v>
       </c>
       <c r="L84" t="n">
-        <v>0.57</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="M84" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="N84" t="n">
-        <v>0.62</v>
+        <v>0.85</v>
       </c>
       <c r="O84" t="n">
         <v>6</v>
@@ -4765,10 +4765,10 @@
         <v>0.7</v>
       </c>
       <c r="H85" t="n">
-        <v>3.48</v>
+        <v>3.58</v>
       </c>
       <c r="I85" t="n">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
       <c r="J85" t="n">
         <v>2</v>
@@ -4777,13 +4777,13 @@
         <v>0</v>
       </c>
       <c r="L85" t="n">
-        <v>0.43</v>
+        <v>0.53</v>
       </c>
       <c r="M85" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="N85" t="n">
-        <v>0.48</v>
+        <v>0.53</v>
       </c>
       <c r="O85" t="n">
         <v>1</v>
@@ -4816,28 +4816,28 @@
         <v>0.8100000000000001</v>
       </c>
       <c r="H86" t="n">
-        <v>4.56</v>
+        <v>4.13</v>
       </c>
       <c r="I86" t="n">
-        <v>0.96</v>
+        <v>0.97</v>
       </c>
       <c r="J86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K86" t="n">
         <v>0</v>
       </c>
       <c r="L86" t="n">
-        <v>0.82</v>
+        <v>0.39</v>
       </c>
       <c r="M86" t="n">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="N86" t="n">
-        <v>0.97</v>
+        <v>0.55</v>
       </c>
       <c r="O86" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87">
@@ -4867,10 +4867,10 @@
         <v>2.07</v>
       </c>
       <c r="H87" t="n">
-        <v>3.55</v>
+        <v>3.78</v>
       </c>
       <c r="I87" t="n">
-        <v>1.58</v>
+        <v>1.57</v>
       </c>
       <c r="J87" t="n">
         <v>2</v>
@@ -4879,13 +4879,13 @@
         <v>1</v>
       </c>
       <c r="L87" t="n">
-        <v>0.54</v>
+        <v>0.77</v>
       </c>
       <c r="M87" t="n">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="N87" t="n">
-        <v>1.03</v>
+        <v>1.27</v>
       </c>
       <c r="O87" t="n">
         <v>5</v>
@@ -4918,10 +4918,10 @@
         <v>0.28</v>
       </c>
       <c r="H88" t="n">
-        <v>2.36</v>
+        <v>2.71</v>
       </c>
       <c r="I88" t="n">
-        <v>0.17</v>
+        <v>0.21</v>
       </c>
       <c r="J88" t="n">
         <v>1</v>
@@ -4930,13 +4930,13 @@
         <v>0</v>
       </c>
       <c r="L88" t="n">
-        <v>0.18</v>
+        <v>0.53</v>
       </c>
       <c r="M88" t="n">
-        <v>0.11</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="N88" t="n">
-        <v>0.29</v>
+        <v>0.61</v>
       </c>
       <c r="O88" t="n">
         <v>2</v>
@@ -4969,10 +4969,10 @@
         <v>0.45</v>
       </c>
       <c r="H89" t="n">
-        <v>0.8</v>
+        <v>1.01</v>
       </c>
       <c r="I89" t="n">
-        <v>0.6</v>
+        <v>0.55</v>
       </c>
       <c r="J89" t="n">
         <v>0</v>
@@ -4981,13 +4981,13 @@
         <v>0</v>
       </c>
       <c r="L89" t="n">
-        <v>0.34</v>
+        <v>0.13</v>
       </c>
       <c r="M89" t="n">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="N89" t="n">
-        <v>0.49</v>
+        <v>0.23</v>
       </c>
       <c r="O89" t="n">
         <v>4</v>
@@ -5020,10 +5020,10 @@
         <v>0.2</v>
       </c>
       <c r="H90" t="n">
-        <v>1.55</v>
+        <v>1.54</v>
       </c>
       <c r="I90" t="n">
-        <v>0.19</v>
+        <v>0.27</v>
       </c>
       <c r="J90" t="n">
         <v>1</v>
@@ -5032,13 +5032,13 @@
         <v>0</v>
       </c>
       <c r="L90" t="n">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="M90" t="n">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="N90" t="n">
-        <v>0.2</v>
+        <v>0.27</v>
       </c>
       <c r="O90" t="n">
         <v>1</v>
@@ -5074,7 +5074,7 @@
         <v>0.86</v>
       </c>
       <c r="I91" t="n">
-        <v>1.01</v>
+        <v>1.27</v>
       </c>
       <c r="J91" t="n">
         <v>0</v>
@@ -5086,10 +5086,10 @@
         <v>0.05</v>
       </c>
       <c r="M91" t="n">
-        <v>0.14</v>
+        <v>0.4</v>
       </c>
       <c r="N91" t="n">
-        <v>0.19</v>
+        <v>0.45</v>
       </c>
       <c r="O91" t="n">
         <v>2</v>
@@ -5122,10 +5122,10 @@
         <v>0.29</v>
       </c>
       <c r="H92" t="n">
-        <v>1.3</v>
+        <v>1.12</v>
       </c>
       <c r="I92" t="n">
-        <v>0.21</v>
+        <v>0.26</v>
       </c>
       <c r="J92" t="n">
         <v>0</v>
@@ -5134,13 +5134,13 @@
         <v>0</v>
       </c>
       <c r="L92" t="n">
-        <v>0.38</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="M92" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
       <c r="N92" t="n">
-        <v>0.46</v>
+        <v>0.59</v>
       </c>
       <c r="O92" t="n">
         <v>1</v>
@@ -5173,10 +5173,10 @@
         <v>1.13</v>
       </c>
       <c r="H93" t="n">
-        <v>0.88</v>
+        <v>0.82</v>
       </c>
       <c r="I93" t="n">
-        <v>1</v>
+        <v>0.97</v>
       </c>
       <c r="J93" t="n">
         <v>0</v>
@@ -5185,13 +5185,13 @@
         <v>0</v>
       </c>
       <c r="L93" t="n">
-        <v>0.19</v>
+        <v>0.13</v>
       </c>
       <c r="M93" t="n">
-        <v>0.13</v>
+        <v>0.16</v>
       </c>
       <c r="N93" t="n">
-        <v>0.33</v>
+        <v>0.29</v>
       </c>
       <c r="O93" t="n">
         <v>2</v>
@@ -5224,10 +5224,10 @@
         <v>0.11</v>
       </c>
       <c r="H94" t="n">
-        <v>1.12</v>
+        <v>1.11</v>
       </c>
       <c r="I94" t="n">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="J94" t="n">
         <v>0</v>
@@ -5236,13 +5236,13 @@
         <v>0</v>
       </c>
       <c r="L94" t="n">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="M94" t="n">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="N94" t="n">
-        <v>0.14</v>
+        <v>0.16</v>
       </c>
       <c r="O94" t="n">
         <v>2</v>
@@ -5275,10 +5275,10 @@
         <v>1.12</v>
       </c>
       <c r="H95" t="n">
-        <v>0.41</v>
+        <v>0.46</v>
       </c>
       <c r="I95" t="n">
-        <v>0.93</v>
+        <v>1.45</v>
       </c>
       <c r="J95" t="n">
         <v>0</v>
@@ -5287,13 +5287,13 @@
         <v>0</v>
       </c>
       <c r="L95" t="n">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="M95" t="n">
-        <v>0.19</v>
+        <v>0.33</v>
       </c>
       <c r="N95" t="n">
-        <v>0.34</v>
+        <v>0.53</v>
       </c>
       <c r="O95" t="n">
         <v>3</v>
@@ -5326,28 +5326,28 @@
         <v>1.21</v>
       </c>
       <c r="H96" t="n">
-        <v>2.22</v>
+        <v>2.5</v>
       </c>
       <c r="I96" t="n">
-        <v>0.99</v>
+        <v>1.08</v>
       </c>
       <c r="J96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K96" t="n">
         <v>0</v>
       </c>
       <c r="L96" t="n">
-        <v>0.33</v>
+        <v>0.05</v>
       </c>
       <c r="M96" t="n">
-        <v>0.22</v>
+        <v>0.13</v>
       </c>
       <c r="N96" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.18</v>
       </c>
       <c r="O96" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="97">
@@ -5377,10 +5377,10 @@
         <v>0.89</v>
       </c>
       <c r="H97" t="n">
-        <v>2.26</v>
+        <v>2.4</v>
       </c>
       <c r="I97" t="n">
-        <v>0.99</v>
+        <v>1.21</v>
       </c>
       <c r="J97" t="n">
         <v>2</v>
@@ -5389,13 +5389,13 @@
         <v>0</v>
       </c>
       <c r="L97" t="n">
-        <v>0.13</v>
+        <v>0.01</v>
       </c>
       <c r="M97" t="n">
-        <v>0.1</v>
+        <v>0.32</v>
       </c>
       <c r="N97" t="n">
-        <v>0.24</v>
+        <v>0.32</v>
       </c>
       <c r="O97" t="n">
         <v>3</v>
@@ -5431,7 +5431,7 @@
         <v>0.76</v>
       </c>
       <c r="I98" t="n">
-        <v>3.14</v>
+        <v>3.12</v>
       </c>
       <c r="J98" t="n">
         <v>0</v>
@@ -5443,10 +5443,10 @@
         <v>0.31</v>
       </c>
       <c r="M98" t="n">
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
       <c r="N98" t="n">
-        <v>0.37</v>
+        <v>0.39</v>
       </c>
       <c r="O98" t="n">
         <v>4</v>
@@ -5479,10 +5479,10 @@
         <v>0.47</v>
       </c>
       <c r="H99" t="n">
-        <v>1.02</v>
+        <v>1.22</v>
       </c>
       <c r="I99" t="n">
-        <v>0.66</v>
+        <v>0.63</v>
       </c>
       <c r="J99" t="n">
         <v>0</v>
@@ -5491,13 +5491,13 @@
         <v>0</v>
       </c>
       <c r="L99" t="n">
-        <v>0.08</v>
+        <v>0.28</v>
       </c>
       <c r="M99" t="n">
-        <v>0.19</v>
+        <v>0.16</v>
       </c>
       <c r="N99" t="n">
-        <v>0.26</v>
+        <v>0.44</v>
       </c>
       <c r="O99" t="n">
         <v>1</v>
@@ -5530,10 +5530,10 @@
         <v>0.21</v>
       </c>
       <c r="H100" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.54</v>
       </c>
       <c r="I100" t="n">
-        <v>0.26</v>
+        <v>0.19</v>
       </c>
       <c r="J100" t="n">
         <v>0</v>
@@ -5542,13 +5542,13 @@
         <v>0</v>
       </c>
       <c r="L100" t="n">
-        <v>0.31</v>
+        <v>0.09</v>
       </c>
       <c r="M100" t="n">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="N100" t="n">
-        <v>0.37</v>
+        <v>0.12</v>
       </c>
       <c r="O100" t="n">
         <v>1</v>
@@ -5584,7 +5584,7 @@
         <v>1.67</v>
       </c>
       <c r="I101" t="n">
-        <v>0.68</v>
+        <v>0.63</v>
       </c>
       <c r="J101" t="n">
         <v>0</v>
@@ -5596,10 +5596,10 @@
         <v>0.22</v>
       </c>
       <c r="M101" t="n">
-        <v>0.06</v>
+        <v>0.11</v>
       </c>
       <c r="N101" t="n">
-        <v>0.27</v>
+        <v>0.33</v>
       </c>
       <c r="O101" t="n">
         <v>1</v>
@@ -5632,10 +5632,10 @@
         <v>2.54</v>
       </c>
       <c r="H102" t="n">
-        <v>0.76</v>
+        <v>0.82</v>
       </c>
       <c r="I102" t="n">
-        <v>1.6</v>
+        <v>1.88</v>
       </c>
       <c r="J102" t="n">
         <v>0</v>
@@ -5644,13 +5644,13 @@
         <v>0</v>
       </c>
       <c r="L102" t="n">
-        <v>0.45</v>
+        <v>0.39</v>
       </c>
       <c r="M102" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.66</v>
       </c>
       <c r="N102" t="n">
-        <v>1.39</v>
+        <v>1.05</v>
       </c>
       <c r="O102" t="n">
         <v>1</v>
@@ -5683,10 +5683,10 @@
         <v>1.29</v>
       </c>
       <c r="H103" t="n">
-        <v>0.74</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="I103" t="n">
-        <v>1.46</v>
+        <v>1.44</v>
       </c>
       <c r="J103" t="n">
         <v>0</v>
@@ -5695,13 +5695,13 @@
         <v>0</v>
       </c>
       <c r="L103" t="n">
-        <v>0.14</v>
+        <v>0.09</v>
       </c>
       <c r="M103" t="n">
-        <v>0.17</v>
+        <v>0.15</v>
       </c>
       <c r="N103" t="n">
-        <v>0.31</v>
+        <v>0.24</v>
       </c>
       <c r="O103" t="n">
         <v>2</v>
@@ -5734,10 +5734,10 @@
         <v>1.8</v>
       </c>
       <c r="H104" t="n">
-        <v>0.95</v>
+        <v>0.84</v>
       </c>
       <c r="I104" t="n">
-        <v>2.68</v>
+        <v>2.5</v>
       </c>
       <c r="J104" t="n">
         <v>0</v>
@@ -5746,13 +5746,13 @@
         <v>2</v>
       </c>
       <c r="L104" t="n">
-        <v>0.17</v>
+        <v>0.28</v>
       </c>
       <c r="M104" t="n">
-        <v>0.88</v>
+        <v>0.7</v>
       </c>
       <c r="N104" t="n">
-        <v>1.04</v>
+        <v>0.98</v>
       </c>
       <c r="O104" t="n">
         <v>3</v>
@@ -5785,28 +5785,28 @@
         <v>1.07</v>
       </c>
       <c r="H105" t="n">
-        <v>2.02</v>
+        <v>2.58</v>
       </c>
       <c r="I105" t="n">
-        <v>1.02</v>
+        <v>1.08</v>
       </c>
       <c r="J105" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K105" t="n">
         <v>0</v>
       </c>
       <c r="L105" t="n">
-        <v>0.36</v>
+        <v>0.2</v>
       </c>
       <c r="M105" t="n">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="N105" t="n">
-        <v>0.41</v>
+        <v>0.21</v>
       </c>
       <c r="O105" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106">
@@ -5836,10 +5836,10 @@
         <v>1.19</v>
       </c>
       <c r="H106" t="n">
-        <v>0.74</v>
+        <v>0.8</v>
       </c>
       <c r="I106" t="n">
-        <v>1.6</v>
+        <v>1.42</v>
       </c>
       <c r="J106" t="n">
         <v>0</v>
@@ -5851,10 +5851,10 @@
         <v>0.03</v>
       </c>
       <c r="M106" t="n">
-        <v>0.41</v>
+        <v>0.23</v>
       </c>
       <c r="N106" t="n">
-        <v>0.44</v>
+        <v>0.25</v>
       </c>
       <c r="O106" t="n">
         <v>3</v>
@@ -5887,10 +5887,10 @@
         <v>0.6</v>
       </c>
       <c r="H107" t="n">
-        <v>0.55</v>
+        <v>0.68</v>
       </c>
       <c r="I107" t="n">
-        <v>0.3</v>
+        <v>0.39</v>
       </c>
       <c r="J107" t="n">
         <v>0</v>
@@ -5899,13 +5899,13 @@
         <v>0</v>
       </c>
       <c r="L107" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
       <c r="M107" t="n">
-        <v>0.3</v>
+        <v>0.21</v>
       </c>
       <c r="N107" t="n">
-        <v>0.33</v>
+        <v>0.31</v>
       </c>
       <c r="O107" t="n">
         <v>1</v>
@@ -5938,10 +5938,10 @@
         <v>0.4</v>
       </c>
       <c r="H108" t="n">
-        <v>0.7</v>
+        <v>0.77</v>
       </c>
       <c r="I108" t="n">
-        <v>0.51</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="J108" t="n">
         <v>0</v>
@@ -5950,13 +5950,13 @@
         <v>0</v>
       </c>
       <c r="L108" t="n">
-        <v>0.09</v>
+        <v>0.16</v>
       </c>
       <c r="M108" t="n">
-        <v>0.11</v>
+        <v>0.16</v>
       </c>
       <c r="N108" t="n">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="O108" t="n">
         <v>1</v>
@@ -5989,28 +5989,28 @@
         <v>0.26</v>
       </c>
       <c r="H109" t="n">
-        <v>3.43</v>
+        <v>3.28</v>
       </c>
       <c r="I109" t="n">
-        <v>0.25</v>
+        <v>0.26</v>
       </c>
       <c r="J109" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K109" t="n">
         <v>0</v>
       </c>
       <c r="L109" t="n">
-        <v>0.47</v>
+        <v>0.32</v>
       </c>
       <c r="M109" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="N109" t="n">
-        <v>0.47</v>
+        <v>0.32</v>
       </c>
       <c r="O109" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110">
@@ -6040,10 +6040,10 @@
         <v>1.45</v>
       </c>
       <c r="H110" t="n">
-        <v>0.82</v>
+        <v>0.97</v>
       </c>
       <c r="I110" t="n">
-        <v>0.91</v>
+        <v>1.07</v>
       </c>
       <c r="J110" t="n">
         <v>0</v>
@@ -6052,13 +6052,13 @@
         <v>0</v>
       </c>
       <c r="L110" t="n">
-        <v>0.29</v>
+        <v>0.14</v>
       </c>
       <c r="M110" t="n">
-        <v>0.54</v>
+        <v>0.38</v>
       </c>
       <c r="N110" t="n">
-        <v>0.83</v>
+        <v>0.52</v>
       </c>
       <c r="O110" t="n">
         <v>1</v>
@@ -6091,25 +6091,25 @@
         <v>1.39</v>
       </c>
       <c r="H111" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="I111" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="J111" t="n">
+        <v>0</v>
+      </c>
+      <c r="K111" t="n">
+        <v>0</v>
+      </c>
+      <c r="L111" t="n">
         <v>0.43</v>
       </c>
-      <c r="I111" t="n">
-        <v>1.34</v>
-      </c>
-      <c r="J111" t="n">
-        <v>0</v>
-      </c>
-      <c r="K111" t="n">
-        <v>0</v>
-      </c>
-      <c r="L111" t="n">
-        <v>0.49</v>
-      </c>
       <c r="M111" t="n">
-        <v>0.05</v>
+        <v>0.19</v>
       </c>
       <c r="N111" t="n">
-        <v>0.54</v>
+        <v>0.62</v>
       </c>
       <c r="O111" t="n">
         <v>2</v>
@@ -6142,25 +6142,25 @@
         <v>0.59</v>
       </c>
       <c r="H112" t="n">
-        <v>2.23</v>
+        <v>2.15</v>
       </c>
       <c r="I112" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="J112" t="n">
+        <v>0</v>
+      </c>
+      <c r="K112" t="n">
+        <v>0</v>
+      </c>
+      <c r="L112" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="M112" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="N112" t="n">
         <v>0.77</v>
-      </c>
-      <c r="J112" t="n">
-        <v>0</v>
-      </c>
-      <c r="K112" t="n">
-        <v>0</v>
-      </c>
-      <c r="L112" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="M112" t="n">
-        <v>0.18</v>
-      </c>
-      <c r="N112" t="n">
-        <v>0.83</v>
       </c>
       <c r="O112" t="n">
         <v>2</v>
@@ -6193,10 +6193,10 @@
         <v>3.38</v>
       </c>
       <c r="H113" t="n">
-        <v>1.49</v>
+        <v>1.4</v>
       </c>
       <c r="I113" t="n">
-        <v>2.03</v>
+        <v>2.12</v>
       </c>
       <c r="J113" t="n">
         <v>0</v>
@@ -6205,13 +6205,13 @@
         <v>1</v>
       </c>
       <c r="L113" t="n">
-        <v>0.21</v>
+        <v>0.3</v>
       </c>
       <c r="M113" t="n">
-        <v>1.35</v>
+        <v>1.26</v>
       </c>
       <c r="N113" t="n">
-        <v>1.57</v>
+        <v>1.56</v>
       </c>
       <c r="O113" t="n">
         <v>5</v>
@@ -6244,10 +6244,10 @@
         <v>0.42</v>
       </c>
       <c r="H114" t="n">
-        <v>1.16</v>
+        <v>1.2</v>
       </c>
       <c r="I114" t="n">
-        <v>0.5</v>
+        <v>0.36</v>
       </c>
       <c r="J114" t="n">
         <v>0</v>
@@ -6256,13 +6256,13 @@
         <v>0</v>
       </c>
       <c r="L114" t="n">
-        <v>0.62</v>
+        <v>0.58</v>
       </c>
       <c r="M114" t="n">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
       <c r="N114" t="n">
-        <v>0.7</v>
+        <v>0.63</v>
       </c>
       <c r="O114" t="n">
         <v>2</v>
@@ -6295,10 +6295,10 @@
         <v>1.02</v>
       </c>
       <c r="H115" t="n">
-        <v>0.96</v>
+        <v>1.06</v>
       </c>
       <c r="I115" t="n">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
       <c r="J115" t="n">
         <v>0</v>
@@ -6307,13 +6307,13 @@
         <v>0</v>
       </c>
       <c r="L115" t="n">
-        <v>0.16</v>
+        <v>0.26</v>
       </c>
       <c r="M115" t="n">
-        <v>0.32</v>
+        <v>0.37</v>
       </c>
       <c r="N115" t="n">
-        <v>0.47</v>
+        <v>0.63</v>
       </c>
       <c r="O115" t="n">
         <v>3</v>
@@ -6346,10 +6346,10 @@
         <v>0.84</v>
       </c>
       <c r="H116" t="n">
-        <v>0.91</v>
+        <v>0.93</v>
       </c>
       <c r="I116" t="n">
-        <v>0.93</v>
+        <v>1.01</v>
       </c>
       <c r="J116" t="n">
         <v>0</v>
@@ -6358,13 +6358,13 @@
         <v>0</v>
       </c>
       <c r="L116" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="M116" t="n">
-        <v>0.09</v>
+        <v>0.17</v>
       </c>
       <c r="N116" t="n">
-        <v>0.1</v>
+        <v>0.19</v>
       </c>
       <c r="O116" t="n">
         <v>3</v>
@@ -6397,10 +6397,10 @@
         <v>0.44</v>
       </c>
       <c r="H117" t="n">
-        <v>1.99</v>
+        <v>1.88</v>
       </c>
       <c r="I117" t="n">
-        <v>0.62</v>
+        <v>0.59</v>
       </c>
       <c r="J117" t="n">
         <v>0</v>
@@ -6409,13 +6409,13 @@
         <v>0</v>
       </c>
       <c r="L117" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="M117" t="n">
-        <v>0.18</v>
+        <v>0.15</v>
       </c>
       <c r="N117" t="n">
-        <v>0.23</v>
+        <v>0.22</v>
       </c>
       <c r="O117" t="n">
         <v>4</v>
@@ -6448,10 +6448,10 @@
         <v>0.6899999999999999</v>
       </c>
       <c r="H118" t="n">
-        <v>1.62</v>
+        <v>1.69</v>
       </c>
       <c r="I118" t="n">
-        <v>1.01</v>
+        <v>1.08</v>
       </c>
       <c r="J118" t="n">
         <v>1</v>
@@ -6460,13 +6460,13 @@
         <v>1</v>
       </c>
       <c r="L118" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.14</v>
       </c>
       <c r="M118" t="n">
-        <v>0.32</v>
+        <v>0.39</v>
       </c>
       <c r="N118" t="n">
-        <v>0.39</v>
+        <v>0.53</v>
       </c>
       <c r="O118" t="n">
         <v>0</v>
@@ -6499,10 +6499,10 @@
         <v>1.61</v>
       </c>
       <c r="H119" t="n">
-        <v>0.84</v>
+        <v>0.98</v>
       </c>
       <c r="I119" t="n">
-        <v>0.92</v>
+        <v>1.07</v>
       </c>
       <c r="J119" t="n">
         <v>0</v>
@@ -6511,13 +6511,13 @@
         <v>0</v>
       </c>
       <c r="L119" t="n">
-        <v>0.12</v>
+        <v>0.02</v>
       </c>
       <c r="M119" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.54</v>
       </c>
       <c r="N119" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="O119" t="n">
         <v>1</v>
@@ -6550,10 +6550,10 @@
         <v>1.68</v>
       </c>
       <c r="H120" t="n">
-        <v>0.97</v>
+        <v>0.89</v>
       </c>
       <c r="I120" t="n">
-        <v>1.96</v>
+        <v>2.09</v>
       </c>
       <c r="J120" t="n">
         <v>0</v>
@@ -6562,13 +6562,13 @@
         <v>1</v>
       </c>
       <c r="L120" t="n">
-        <v>0.35</v>
+        <v>0.43</v>
       </c>
       <c r="M120" t="n">
-        <v>0.28</v>
+        <v>0.41</v>
       </c>
       <c r="N120" t="n">
-        <v>0.63</v>
+        <v>0.84</v>
       </c>
       <c r="O120" t="n">
         <v>4</v>
@@ -6601,25 +6601,25 @@
         <v>3.23</v>
       </c>
       <c r="H121" t="n">
-        <v>0.54</v>
+        <v>0.65</v>
       </c>
       <c r="I121" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="J121" t="n">
+        <v>0</v>
+      </c>
+      <c r="K121" t="n">
+        <v>0</v>
+      </c>
+      <c r="L121" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="M121" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="N121" t="n">
         <v>1.71</v>
-      </c>
-      <c r="J121" t="n">
-        <v>0</v>
-      </c>
-      <c r="K121" t="n">
-        <v>0</v>
-      </c>
-      <c r="L121" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="M121" t="n">
-        <v>1.52</v>
-      </c>
-      <c r="N121" t="n">
-        <v>1.56</v>
       </c>
       <c r="O121" t="n">
         <v>5</v>
@@ -6652,10 +6652,10 @@
         <v>0.4</v>
       </c>
       <c r="H122" t="n">
-        <v>0.27</v>
+        <v>0.33</v>
       </c>
       <c r="I122" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="J122" t="n">
         <v>0</v>
@@ -6667,10 +6667,10 @@
         <v>0.03</v>
       </c>
       <c r="M122" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="N122" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="O122" t="n">
         <v>0</v>
@@ -6703,10 +6703,10 @@
         <v>2.75</v>
       </c>
       <c r="H123" t="n">
-        <v>0.57</v>
+        <v>0.55</v>
       </c>
       <c r="I123" t="n">
-        <v>2.32</v>
+        <v>2.72</v>
       </c>
       <c r="J123" t="n">
         <v>0</v>
@@ -6715,13 +6715,13 @@
         <v>1</v>
       </c>
       <c r="L123" t="n">
-        <v>0.18</v>
+        <v>0.2</v>
       </c>
       <c r="M123" t="n">
-        <v>0.43</v>
+        <v>0.03</v>
       </c>
       <c r="N123" t="n">
-        <v>0.61</v>
+        <v>0.23</v>
       </c>
       <c r="O123" t="n">
         <v>3</v>
@@ -6754,10 +6754,10 @@
         <v>0.8100000000000001</v>
       </c>
       <c r="H124" t="n">
-        <v>0.88</v>
+        <v>0.97</v>
       </c>
       <c r="I124" t="n">
-        <v>1.1</v>
+        <v>1.19</v>
       </c>
       <c r="J124" t="n">
         <v>0</v>
@@ -6766,10 +6766,10 @@
         <v>0</v>
       </c>
       <c r="L124" t="n">
-        <v>0.34</v>
+        <v>0.25</v>
       </c>
       <c r="M124" t="n">
-        <v>0.29</v>
+        <v>0.38</v>
       </c>
       <c r="N124" t="n">
         <v>0.63</v>
@@ -6805,10 +6805,10 @@
         <v>3.01</v>
       </c>
       <c r="H125" t="n">
-        <v>1.6</v>
+        <v>1.71</v>
       </c>
       <c r="I125" t="n">
-        <v>2.65</v>
+        <v>2.93</v>
       </c>
       <c r="J125" t="n">
         <v>0</v>
@@ -6817,13 +6817,13 @@
         <v>2</v>
       </c>
       <c r="L125" t="n">
-        <v>0.16</v>
+        <v>0.05</v>
       </c>
       <c r="M125" t="n">
-        <v>0.36</v>
+        <v>0.08</v>
       </c>
       <c r="N125" t="n">
-        <v>0.52</v>
+        <v>0.13</v>
       </c>
       <c r="O125" t="n">
         <v>2</v>
@@ -6856,10 +6856,10 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="H126" t="n">
-        <v>2</v>
+        <v>1.99</v>
       </c>
       <c r="I126" t="n">
-        <v>0.12</v>
+        <v>0.15</v>
       </c>
       <c r="J126" t="n">
         <v>1</v>
@@ -6868,13 +6868,13 @@
         <v>0</v>
       </c>
       <c r="L126" t="n">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="M126" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="N126" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
       <c r="O126" t="n">
         <v>2</v>
@@ -6907,7 +6907,7 @@
         <v>0.58</v>
       </c>
       <c r="H127" t="n">
-        <v>1.95</v>
+        <v>1.73</v>
       </c>
       <c r="I127" t="n">
         <v>0.5</v>
@@ -6919,13 +6919,13 @@
         <v>0</v>
       </c>
       <c r="L127" t="n">
-        <v>0.03</v>
+        <v>0.25</v>
       </c>
       <c r="M127" t="n">
         <v>0.08</v>
       </c>
       <c r="N127" t="n">
-        <v>0.11</v>
+        <v>0.33</v>
       </c>
       <c r="O127" t="n">
         <v>0</v>
@@ -6958,10 +6958,10 @@
         <v>0.88</v>
       </c>
       <c r="H128" t="n">
-        <v>1.11</v>
+        <v>1.33</v>
       </c>
       <c r="I128" t="n">
-        <v>0.66</v>
+        <v>0.7</v>
       </c>
       <c r="J128" t="n">
         <v>0</v>
@@ -6970,13 +6970,13 @@
         <v>0</v>
       </c>
       <c r="L128" t="n">
-        <v>0.06</v>
+        <v>0.28</v>
       </c>
       <c r="M128" t="n">
-        <v>0.22</v>
+        <v>0.18</v>
       </c>
       <c r="N128" t="n">
-        <v>0.27</v>
+        <v>0.47</v>
       </c>
       <c r="O128" t="n">
         <v>2</v>
@@ -7009,10 +7009,10 @@
         <v>0.83</v>
       </c>
       <c r="H129" t="n">
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
       <c r="I129" t="n">
-        <v>1.19</v>
+        <v>1.34</v>
       </c>
       <c r="J129" t="n">
         <v>0</v>
@@ -7021,13 +7021,13 @@
         <v>0</v>
       </c>
       <c r="L129" t="n">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
       <c r="M129" t="n">
-        <v>0.36</v>
+        <v>0.51</v>
       </c>
       <c r="N129" t="n">
-        <v>0.43</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="O129" t="n">
         <v>2</v>
@@ -7060,27 +7060,486 @@
         <v>0.7</v>
       </c>
       <c r="H130" t="n">
-        <v>1.93</v>
+        <v>1.77</v>
       </c>
       <c r="I130" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="J130" t="n">
+        <v>0</v>
+      </c>
+      <c r="K130" t="n">
+        <v>0</v>
+      </c>
+      <c r="L130" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="M130" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="N130" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="O130" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Hellas Verona</t>
+        </is>
+      </c>
+      <c r="D131" t="n">
+        <v>1</v>
+      </c>
+      <c r="E131" t="n">
+        <v>0</v>
+      </c>
+      <c r="F131" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="G131" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="H131" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="I131" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="J131" t="n">
+        <v>0</v>
+      </c>
+      <c r="K131" t="n">
+        <v>0</v>
+      </c>
+      <c r="L131" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="M131" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="N131" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="O131" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Bologna</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Venezia</t>
+        </is>
+      </c>
+      <c r="D132" t="n">
+        <v>3</v>
+      </c>
+      <c r="E132" t="n">
+        <v>0</v>
+      </c>
+      <c r="F132" t="n">
+        <v>3.22</v>
+      </c>
+      <c r="G132" t="n">
         <v>0.44</v>
       </c>
-      <c r="J130" t="n">
-        <v>1</v>
-      </c>
-      <c r="K130" t="n">
-        <v>0</v>
-      </c>
-      <c r="L130" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="M130" t="n">
+      <c r="H132" t="n">
+        <v>3.26</v>
+      </c>
+      <c r="I132" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="J132" t="n">
+        <v>2</v>
+      </c>
+      <c r="K132" t="n">
+        <v>0</v>
+      </c>
+      <c r="L132" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="M132" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="N132" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="O132" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Como</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Monza</t>
+        </is>
+      </c>
+      <c r="D133" t="n">
+        <v>1</v>
+      </c>
+      <c r="E133" t="n">
+        <v>1</v>
+      </c>
+      <c r="F133" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="G133" t="n">
+        <v>1.34</v>
+      </c>
+      <c r="H133" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="I133" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="J133" t="n">
+        <v>0</v>
+      </c>
+      <c r="K133" t="n">
+        <v>1</v>
+      </c>
+      <c r="L133" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="M133" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="N133" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="O133" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Milan</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Empoli</t>
+        </is>
+      </c>
+      <c r="D134" t="n">
+        <v>3</v>
+      </c>
+      <c r="E134" t="n">
+        <v>0</v>
+      </c>
+      <c r="F134" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="G134" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="H134" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="I134" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="J134" t="n">
+        <v>0</v>
+      </c>
+      <c r="K134" t="n">
+        <v>0</v>
+      </c>
+      <c r="L134" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="M134" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N134" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="O134" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Lecce</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Juventus</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>1</v>
+      </c>
+      <c r="E135" t="n">
+        <v>1</v>
+      </c>
+      <c r="F135" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="G135" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="H135" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="I135" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="J135" t="n">
+        <v>0</v>
+      </c>
+      <c r="K135" t="n">
+        <v>1</v>
+      </c>
+      <c r="L135" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="M135" t="n">
         <v>0.26</v>
       </c>
-      <c r="N130" t="n">
-        <v>1.06</v>
-      </c>
-      <c r="O130" t="n">
+      <c r="N135" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="O135" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Parma</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>Lazio</t>
+        </is>
+      </c>
+      <c r="D136" t="n">
+        <v>3</v>
+      </c>
+      <c r="E136" t="n">
+        <v>1</v>
+      </c>
+      <c r="F136" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="G136" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="H136" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="I136" t="n">
+        <v>2.48</v>
+      </c>
+      <c r="J136" t="n">
+        <v>0</v>
+      </c>
+      <c r="K136" t="n">
+        <v>0</v>
+      </c>
+      <c r="L136" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="M136" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="N136" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="O136" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Torino</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>Napoli</t>
+        </is>
+      </c>
+      <c r="D137" t="n">
+        <v>0</v>
+      </c>
+      <c r="E137" t="n">
+        <v>1</v>
+      </c>
+      <c r="F137" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="G137" t="n">
+        <v>1.41</v>
+      </c>
+      <c r="H137" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="I137" t="n">
+        <v>2.01</v>
+      </c>
+      <c r="J137" t="n">
+        <v>0</v>
+      </c>
+      <c r="K137" t="n">
+        <v>0</v>
+      </c>
+      <c r="L137" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M137" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="N137" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="O137" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Udinese</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Genoa</t>
+        </is>
+      </c>
+      <c r="D138" t="n">
+        <v>0</v>
+      </c>
+      <c r="E138" t="n">
+        <v>2</v>
+      </c>
+      <c r="F138" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="G138" t="n">
+        <v>1.64</v>
+      </c>
+      <c r="H138" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="I138" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="J138" t="n">
+        <v>0</v>
+      </c>
+      <c r="K138" t="n">
+        <v>0</v>
+      </c>
+      <c r="L138" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="M138" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="N138" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="O138" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Roma</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Atalanta</t>
+        </is>
+      </c>
+      <c r="D139" t="n">
+        <v>0</v>
+      </c>
+      <c r="E139" t="n">
+        <v>2</v>
+      </c>
+      <c r="F139" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="G139" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="H139" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="I139" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="J139" t="n">
+        <v>0</v>
+      </c>
+      <c r="K139" t="n">
+        <v>0</v>
+      </c>
+      <c r="L139" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="M139" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="N139" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="O139" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>